<commit_message>
Writing new Reading Functions
</commit_message>
<xml_diff>
--- a/cv4DatabaseSarMdac.xlsx
+++ b/cv4DatabaseSarMdac.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:BD10"/>
+  <dimension ref="A1:BD12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -2263,6 +2263,350 @@
         <v>13906</v>
       </c>
     </row>
+    <row r="11">
+      <c r="A11" t="inlineStr">
+        <is>
+          <t>3-9-2022 11:45:20</t>
+        </is>
+      </c>
+      <c r="B11" t="n">
+        <v>60</v>
+      </c>
+      <c r="C11" t="n">
+        <v>169153</v>
+      </c>
+      <c r="D11" t="n">
+        <v>0</v>
+      </c>
+      <c r="E11" t="n">
+        <v>1</v>
+      </c>
+      <c r="F11" t="n">
+        <v>242.2610625</v>
+      </c>
+      <c r="G11" t="n">
+        <v>4339.453375</v>
+      </c>
+      <c r="H11" t="n">
+        <v>4339.4090625</v>
+      </c>
+      <c r="I11" t="n">
+        <v>4338.7996875</v>
+      </c>
+      <c r="J11" t="n">
+        <v>4340.3539375</v>
+      </c>
+      <c r="K11" t="n">
+        <v>4338.75225</v>
+      </c>
+      <c r="L11" t="n">
+        <v>4338.9178125</v>
+      </c>
+      <c r="M11" t="n">
+        <v>4336.4964375</v>
+      </c>
+      <c r="N11" t="n">
+        <v>16.05678125</v>
+      </c>
+      <c r="O11" t="n">
+        <v>23.93606249999999</v>
+      </c>
+      <c r="P11" t="n">
+        <v>31.96037500000001</v>
+      </c>
+      <c r="Q11" t="n">
+        <v>63.58449874999999</v>
+      </c>
+      <c r="R11" t="n">
+        <v>127.1353625</v>
+      </c>
+      <c r="S11" t="n">
+        <v>221.59961</v>
+      </c>
+      <c r="T11" t="n">
+        <v>129.787545</v>
+      </c>
+      <c r="U11" t="n">
+        <v>260.7537975</v>
+      </c>
+      <c r="V11" t="n">
+        <v>390.68310375</v>
+      </c>
+      <c r="W11" t="n">
+        <v>650.8980712499999</v>
+      </c>
+      <c r="X11" t="n">
+        <v>1040.56667625</v>
+      </c>
+      <c r="Y11" t="n">
+        <v>2078.95582625</v>
+      </c>
+      <c r="Z11" t="n">
+        <v>3639.235605</v>
+      </c>
+      <c r="AA11" t="n">
+        <v>10</v>
+      </c>
+      <c r="AB11" t="n">
+        <v>6</v>
+      </c>
+      <c r="AC11" t="n">
+        <v>4</v>
+      </c>
+      <c r="AD11" t="n">
+        <v>2</v>
+      </c>
+      <c r="AE11" t="n">
+        <v>1</v>
+      </c>
+      <c r="AF11" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="AG11" t="n">
+        <v>0.25</v>
+      </c>
+      <c r="AH11" t="n">
+        <v>969</v>
+      </c>
+      <c r="AI11" t="n">
+        <v>18327</v>
+      </c>
+      <c r="AJ11" t="n">
+        <v>35684</v>
+      </c>
+      <c r="AK11" t="n">
+        <v>53040</v>
+      </c>
+      <c r="AL11" t="n">
+        <v>70401</v>
+      </c>
+      <c r="AM11" t="n">
+        <v>87756</v>
+      </c>
+      <c r="AN11" t="n">
+        <v>105112</v>
+      </c>
+      <c r="AO11" t="n">
+        <v>122458</v>
+      </c>
+      <c r="AP11" t="n">
+        <v>23</v>
+      </c>
+      <c r="AQ11" t="n">
+        <v>38</v>
+      </c>
+      <c r="AR11" t="n">
+        <v>61</v>
+      </c>
+      <c r="AS11" t="n">
+        <v>91</v>
+      </c>
+      <c r="AT11" t="n">
+        <v>122</v>
+      </c>
+      <c r="AU11" t="n">
+        <v>243</v>
+      </c>
+      <c r="AV11" t="n">
+        <v>486</v>
+      </c>
+      <c r="AW11" t="n">
+        <v>847</v>
+      </c>
+      <c r="AX11" t="n">
+        <v>496</v>
+      </c>
+      <c r="AY11" t="n">
+        <v>996</v>
+      </c>
+      <c r="AZ11" t="n">
+        <v>1493</v>
+      </c>
+      <c r="BA11" t="n">
+        <v>2487</v>
+      </c>
+      <c r="BB11" t="n">
+        <v>3976</v>
+      </c>
+      <c r="BC11" t="n">
+        <v>7944</v>
+      </c>
+      <c r="BD11" t="n">
+        <v>13906</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="inlineStr">
+        <is>
+          <t>3-9-2022 12:4:11</t>
+        </is>
+      </c>
+      <c r="B12" t="n">
+        <v>61</v>
+      </c>
+      <c r="C12" t="n">
+        <v>169153</v>
+      </c>
+      <c r="D12" t="n">
+        <v>0</v>
+      </c>
+      <c r="E12" t="n">
+        <v>2</v>
+      </c>
+      <c r="F12" t="n">
+        <v>272.0392499999998</v>
+      </c>
+      <c r="G12" t="n">
+        <v>4368.728</v>
+      </c>
+      <c r="H12" t="n">
+        <v>4369.676937499999</v>
+      </c>
+      <c r="I12" t="n">
+        <v>4369.562125</v>
+      </c>
+      <c r="J12" t="n">
+        <v>4371.781</v>
+      </c>
+      <c r="K12" t="n">
+        <v>4369.794625</v>
+      </c>
+      <c r="L12" t="n">
+        <v>4369.190500000001</v>
+      </c>
+      <c r="M12" t="n">
+        <v>4366.098875</v>
+      </c>
+      <c r="N12" t="n">
+        <v>16.01034375</v>
+      </c>
+      <c r="O12" t="n">
+        <v>23.87509375</v>
+      </c>
+      <c r="P12" t="n">
+        <v>32.0115625</v>
+      </c>
+      <c r="Q12" t="n">
+        <v>63.32156249999998</v>
+      </c>
+      <c r="R12" t="n">
+        <v>127.2145625</v>
+      </c>
+      <c r="S12" t="n">
+        <v>221.55065625</v>
+      </c>
+      <c r="T12" t="n">
+        <v>130.41603125</v>
+      </c>
+      <c r="U12" t="n">
+        <v>261.3429062500001</v>
+      </c>
+      <c r="V12" t="n">
+        <v>391.87328125</v>
+      </c>
+      <c r="W12" t="n">
+        <v>652.2020625</v>
+      </c>
+      <c r="X12" t="n">
+        <v>1043.3900625</v>
+      </c>
+      <c r="Y12" t="n">
+        <v>2084.459375</v>
+      </c>
+      <c r="Z12" t="n">
+        <v>3648.59259375</v>
+      </c>
+      <c r="AA12" t="n">
+        <v>10</v>
+      </c>
+      <c r="AB12" t="n">
+        <v>6</v>
+      </c>
+      <c r="AC12" t="n">
+        <v>4</v>
+      </c>
+      <c r="AD12" t="n">
+        <v>2</v>
+      </c>
+      <c r="AE12" t="n">
+        <v>1</v>
+      </c>
+      <c r="AF12" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="AG12" t="n">
+        <v>0.25</v>
+      </c>
+      <c r="AH12" t="n">
+        <v>1088</v>
+      </c>
+      <c r="AI12" t="n">
+        <v>18563</v>
+      </c>
+      <c r="AJ12" t="n">
+        <v>36042</v>
+      </c>
+      <c r="AK12" t="n">
+        <v>53520</v>
+      </c>
+      <c r="AL12" t="n">
+        <v>71007</v>
+      </c>
+      <c r="AM12" t="n">
+        <v>88486</v>
+      </c>
+      <c r="AN12" t="n">
+        <v>105963</v>
+      </c>
+      <c r="AO12" t="n">
+        <v>123427</v>
+      </c>
+      <c r="AP12" t="n">
+        <v>23</v>
+      </c>
+      <c r="AQ12" t="n">
+        <v>38</v>
+      </c>
+      <c r="AR12" t="n">
+        <v>61</v>
+      </c>
+      <c r="AS12" t="n">
+        <v>91</v>
+      </c>
+      <c r="AT12" t="n">
+        <v>122</v>
+      </c>
+      <c r="AU12" t="n">
+        <v>241</v>
+      </c>
+      <c r="AV12" t="n">
+        <v>485</v>
+      </c>
+      <c r="AW12" t="n">
+        <v>844</v>
+      </c>
+      <c r="AX12" t="n">
+        <v>497</v>
+      </c>
+      <c r="AY12" t="n">
+        <v>996</v>
+      </c>
+      <c r="AZ12" t="n">
+        <v>1494</v>
+      </c>
+      <c r="BA12" t="n">
+        <v>2486</v>
+      </c>
+      <c r="BB12" t="n">
+        <v>3977</v>
+      </c>
+      <c r="BC12" t="n">
+        <v>7945</v>
+      </c>
+      <c r="BD12" t="n">
+        <v>13906</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>
 </worksheet>

</xml_diff>